<commit_message>
Update clinic contact create again
</commit_message>
<xml_diff>
--- a/ebs_with_tracing/forms/contact/clinic-create.xlsx
+++ b/ebs_with_tracing/forms/contact/clinic-create.xlsx
@@ -147,7 +147,7 @@
     <t xml:space="preserve">create_new_person</t>
   </si>
   <si>
-    <t xml:space="preserve">Set the Primary Contact UPDATED</t>
+    <t xml:space="preserve">Set the Primary Contact UPDATED AGIN</t>
   </si>
   <si>
     <t xml:space="preserve">प्राथमिक कॉंटॅक्ट चुनें</t>
@@ -6946,7 +6946,7 @@
       </c>
       <c r="C2" s="36" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-09-20  0-04</v>
+        <v>2020-09-20  0-15</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>374</v>

</xml_diff>